<commit_message>
Changed conditional formatting of excel spreadsheet
</commit_message>
<xml_diff>
--- a/RadioVSNED_pos/Diference_CHANGES_NED_POS.xlsx
+++ b/RadioVSNED_pos/Diference_CHANGES_NED_POS.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucashunt/projects/CHANG-ES/RadioVSNED_pos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3112CBA-DFA3-1C4A-B6A5-19D71CFF68AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28400" windowHeight="9100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -235,8 +241,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +303,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -345,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,9 +462,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,6 +514,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,14 +707,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -642,7 +765,7 @@
         <v>2.922713996242682</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -668,7 +791,7 @@
         <v>1.016860760453403</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -691,10 +814,10 @@
         <v>0.75</v>
       </c>
       <c r="H4">
-        <v>0.575919846558283</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.57591984655828299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -714,13 +837,13 @@
         <v>62</v>
       </c>
       <c r="G5">
-        <v>0.00237</v>
+        <v>2.3700000000000001E-3</v>
       </c>
       <c r="H5">
-        <v>0.09230477401105959</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>9.230477401105959E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -743,10 +866,10 @@
         <v>1.25</v>
       </c>
       <c r="H6">
-        <v>0.5823626802886609</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.58236268028866089</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -769,10 +892,10 @@
         <v>0.5</v>
       </c>
       <c r="H7">
-        <v>1.820000000003224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1.8200000000032239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -792,13 +915,13 @@
         <v>65</v>
       </c>
       <c r="G8">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H8">
         <v>1.378433341272197</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -821,10 +944,10 @@
         <v>0.1</v>
       </c>
       <c r="H9">
-        <v>0.1341214166827372</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.13412141668273719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -844,13 +967,13 @@
         <v>67</v>
       </c>
       <c r="G10">
-        <v>0.0053</v>
+        <v>5.3E-3</v>
       </c>
       <c r="H10">
-        <v>0.0297800018949201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>2.97800018949201E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -873,10 +996,10 @@
         <v>0.5</v>
       </c>
       <c r="H11">
-        <v>0.6466841718195618</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0.64668417181956184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -899,10 +1022,10 @@
         <v>0.5</v>
       </c>
       <c r="H12">
-        <v>0.6029902799982322</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>0.60299027999823218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -925,10 +1048,10 @@
         <v>1.25</v>
       </c>
       <c r="H13">
-        <v>1.598731409056728</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>1.5987314090567279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -955,6 +1078,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>$G2+0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>